<commit_message>
Some parameters from 1970 to 2017
</commit_message>
<xml_diff>
--- a/Project 1/StaticParameters/FinalParameters/mean_ps.xlsx
+++ b/Project 1/StaticParameters/FinalParameters/mean_ps.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>97692.14130587083</v>
+        <v>95941.66286295939</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>97477.57906568318</v>
+        <v>95714.4546870803</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>97522.75387542442</v>
+        <v>95796.14810636583</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>97397.2772509074</v>
+        <v>95651.19403706689</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>97702.3711993835</v>
+        <v>95952.93469409621</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>97660.79865940756</v>
+        <v>95899.98587160894</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97538.52001522071</v>
+        <v>95787.18861133493</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>97764.72788900598</v>
+        <v>96010.12640343809</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>97451.45757437767</v>
+        <v>95702.49673202615</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>97502.00490574875</v>
+        <v>95770.74633360193</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>97359.62986769699</v>
+        <v>95625.41423583131</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>97723.29881161457</v>
+        <v>95984.49127048081</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>97546.15572602868</v>
+        <v>95809.35272688311</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>97703.79783397728</v>
+        <v>95956.61864088102</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>97476.05540334857</v>
+        <v>95745.1099113618</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>97527.6167954572</v>
+        <v>95788.00999194197</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>97959.34441992434</v>
+        <v>96213.36815600557</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>97715.39679779885</v>
+        <v>95971.94085414987</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>97427.64814424541</v>
+        <v>95671.19817351598</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>97397.3956445381</v>
+        <v>95656.88068761754</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>97377.89732497316</v>
+        <v>95641.21638272796</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>97626.58432267883</v>
+        <v>95871.59656191245</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>97740.64099051633</v>
+        <v>96001.99221058287</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>97802.68539983607</v>
+        <v>96069.84850926674</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>97503.78387861379</v>
+        <v>95767.5107146684</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>97667.40322561763</v>
+        <v>95928.56803652969</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>97648.10824844865</v>
+        <v>95913.82535589579</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>97474.66942395504</v>
+        <v>95742.96099919418</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>97427.76384802203</v>
+        <v>95684.94771241832</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>97601.06597002693</v>
+        <v>95870.20703733548</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>97716.11506849313</v>
+        <v>95953.78291700241</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>97522.08461538461</v>
+        <v>95803.18162771959</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>97538.97225725093</v>
+        <v>95786.86558448516</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>97665.46229949656</v>
+        <v>95936.17539618588</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>97609.63455684346</v>
+        <v>95892.96180499597</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>97518.54763493738</v>
+        <v>95800.7238248724</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>97729.27111648217</v>
+        <v>95987.95446265939</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>97489.4283573352</v>
+        <v>95750.26768734891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>